<commit_message>
pictures can show now
</commit_message>
<xml_diff>
--- a/CookieOrderSystem/Data/Cookie.xlsx
+++ b/CookieOrderSystem/Data/Cookie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa Kao\Junior\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa Kao\source\repos\CookieOrderSystem\CookieOrderSystem\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18ED08DB-8B5F-4251-9A02-092D4D5AEC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602C58EC-3A4E-48E2-B07C-791080CE7B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{9337E963-1A5D-42BB-8C75-0D6C98FFBEDA}"/>
+    <workbookView xWindow="5760" yWindow="360" windowWidth="17280" windowHeight="8880" xr2:uid="{9337E963-1A5D-42BB-8C75-0D6C98FFBEDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,22 +39,28 @@
     <t>價格</t>
   </si>
   <si>
-    <t>巧克力</t>
-  </si>
-  <si>
-    <t>cookie1.png</t>
-  </si>
-  <si>
-    <t>奶油餅乾</t>
-  </si>
-  <si>
-    <t>cookie2.png</t>
-  </si>
-  <si>
-    <t>燕麥餅</t>
-  </si>
-  <si>
-    <t>cookie3.png</t>
+    <t>愛戀玫瑰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>經典可可</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>經典抹茶</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>classic_cocoa.png</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>classic_matcha.png</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rose_love.png</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -436,7 +442,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -447,7 +453,7 @@
     <col min="4" max="4" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -466,10 +472,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
@@ -483,7 +489,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1">
         <v>8</v>
@@ -494,7 +500,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>

</xml_diff>